<commit_message>
Adding API, UI combination scenarios
</commit_message>
<xml_diff>
--- a/Data Files/data.xlsx
+++ b/Data Files/data.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roshnig\git\KATALON_AutomationPOC\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82E29DC-1E94-4AF2-8BE3-B12CF590B6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65DDD9B-BF23-4E94-8AB9-8D42968EFD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductList" sheetId="1" r:id="rId1"/>
     <sheet name="Customer Registration" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
-    <sheet name="ProductCheckout" sheetId="3" r:id="rId4"/>
-    <sheet name="ProductAdditionAndDelete" sheetId="4" r:id="rId5"/>
+    <sheet name="ProductCheckout" sheetId="3" r:id="rId3"/>
+    <sheet name="ProductAdditionAndDelete" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Pliers</t>
   </si>
@@ -146,6 +145,9 @@
   </si>
   <si>
     <t>Square Ruler,Measuring Tape</t>
+  </si>
+  <si>
+    <t>Austria</t>
   </si>
 </sst>
 </file>
@@ -654,23 +656,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{205957A7-CB4C-4E62-8CBD-AE91D5A83AA9}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C16BCC-257E-490D-B401-6226572EF223}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C16BCC-257E-490D-B401-6226572EF223}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,9 +669,12 @@
     <col min="2" max="2" width="32.33203125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -694,8 +687,17 @@
       <c r="D1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -708,8 +710,17 @@
       <c r="D2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>123456</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2">
+        <v>879456234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -721,6 +732,15 @@
       </c>
       <c r="D3" t="s">
         <v>34</v>
+      </c>
+      <c r="E3">
+        <v>141452</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3">
+        <v>879466234</v>
       </c>
     </row>
   </sheetData>
@@ -732,7 +752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A088A8C4-5457-44B0-AEAD-665185970820}">
   <dimension ref="A1:D2"/>
   <sheetViews>

</xml_diff>